<commit_message>
Excel read and printed all cell value
</commit_message>
<xml_diff>
--- a/EmployeeManagement/TestData/orange_data.xlsx
+++ b/EmployeeManagement/TestData/orange_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JiDi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Company\Maveric C# 2022\AutomationFramework\EmployeeManagement\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>kim123</t>
+  </si>
+  <si>
+    <t>peter</t>
+  </si>
+  <si>
+    <t>peter123</t>
   </si>
 </sst>
 </file>
@@ -368,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -409,6 +415,17 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel Connectivity for Invalid and Add Employee Test
</commit_message>
<xml_diff>
--- a/EmployeeManagement/TestData/orange_data.xlsx
+++ b/EmployeeManagement/TestData/orange_data.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="10063"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="10063" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidLoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="AddValidEmployeeTest" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Username</t>
   </si>
@@ -53,40 +53,40 @@
     <t>kim123</t>
   </si>
   <si>
-    <t>kim124</t>
-  </si>
-  <si>
-    <t>kim125</t>
-  </si>
-  <si>
-    <t>kim126</t>
-  </si>
-  <si>
-    <t>kim127</t>
-  </si>
-  <si>
-    <t>kim128</t>
-  </si>
-  <si>
-    <t>kim129</t>
-  </si>
-  <si>
-    <t>kim130</t>
-  </si>
-  <si>
-    <t>kim131</t>
-  </si>
-  <si>
-    <t>kim132</t>
-  </si>
-  <si>
-    <t>kim133</t>
-  </si>
-  <si>
-    <t>kim134</t>
-  </si>
-  <si>
-    <t>kim135</t>
+    <t>peter</t>
+  </si>
+  <si>
+    <t>peter123</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle Name </t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Expected Employee Name</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>wi</t>
+  </si>
+  <si>
+    <t>wick</t>
+  </si>
+  <si>
+    <t>Jack wick</t>
   </si>
 </sst>
 </file>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C15"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -450,133 +450,12 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -587,12 +466,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="8.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.53515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>